<commit_message>
hoàn thành đọc file template
</commit_message>
<xml_diff>
--- a/WindowsFormsApp1/Files/configamthanh.xlsx
+++ b/WindowsFormsApp1/Files/configamthanh.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngvan\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngvan\source\repos\WindowsFormsApp1\WindowsFormsApp1\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>STT</t>
   </si>
@@ -33,87 +33,45 @@
     <t>File</t>
   </si>
   <si>
-    <t>2100 V/P</t>
-  </si>
-  <si>
     <t>abc.mp3</t>
   </si>
   <si>
-    <t>2000 V/P</t>
-  </si>
-  <si>
     <t>abc.mp4</t>
   </si>
   <si>
-    <t>1900 V/P</t>
-  </si>
-  <si>
     <t>abc.mp5</t>
   </si>
   <si>
-    <t>1800 V/P</t>
-  </si>
-  <si>
     <t>abc.mp6</t>
   </si>
   <si>
-    <t>1700 V/P</t>
-  </si>
-  <si>
     <t>abc.mp7</t>
   </si>
   <si>
-    <t>1600 V/P</t>
-  </si>
-  <si>
     <t>abc.mp8</t>
   </si>
   <si>
-    <t>1500 V/P</t>
-  </si>
-  <si>
     <t>abc.mp9</t>
   </si>
   <si>
-    <t>1400 V/P</t>
-  </si>
-  <si>
     <t>abc.mp10</t>
   </si>
   <si>
-    <t>1300 V/P</t>
-  </si>
-  <si>
     <t>abc.mp11</t>
   </si>
   <si>
-    <t>1200 V/P</t>
-  </si>
-  <si>
     <t>abc.mp12</t>
   </si>
   <si>
-    <t>1100 V/P</t>
-  </si>
-  <si>
     <t>abc.mp13</t>
   </si>
   <si>
-    <t>1000 V/P</t>
-  </si>
-  <si>
     <t>abc.mp14</t>
   </si>
   <si>
-    <t>900 V/P</t>
-  </si>
-  <si>
     <t>abc.mp15</t>
   </si>
   <si>
-    <t>800 V/P</t>
-  </si>
-  <si>
     <t>abc.mp16</t>
   </si>
   <si>
@@ -135,15 +93,9 @@
     <t>abc.mp19</t>
   </si>
   <si>
-    <t>500 V/P Trong m y</t>
-  </si>
-  <si>
     <t>abc.mp20</t>
   </si>
   <si>
-    <t xml:space="preserve">0 V/P STOP </t>
-  </si>
-  <si>
     <t>abc.mp21</t>
   </si>
   <si>
@@ -160,6 +112,78 @@
   </si>
   <si>
     <t>abc.mp25</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2100</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
   </si>
 </sst>
 </file>
@@ -643,8 +667,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -969,14 +996,15 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -994,256 +1022,279 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>